<commit_message>
ScheduleController deve permitir salvar compromissos inconsistentes (#36), testes, mock do valor de 'Now', e alguns refactorings.
App:
- ScheduleController deve permitir salvar compromissos com conflito de horário, em feriados e no passado.
- Método MemberExpressionHelper.GetPropertyDisplayName: pega o display name de uma propriedade de um objeto de model.
- InternalsVisibleTo("CerebelloWebRole.Tests"): permite os testes enxergarem valores dos tipos anônimos retornados pela app.

DB:
- Renomeado Holliday (com "ll") para Holiday (com "l").

Testes:
- Valor de 'Now' nos controllers pode ser mockado.
- Testes para o método Create do ScheduleController: deve permitir salvar compromissos com conflito de horário, em feriados e no passado.
</commit_message>
<xml_diff>
--- a/Specification/Cronograma.xlsx
+++ b/Specification/Cronograma.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="18135" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="18132" windowHeight="7932"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>Tempo</t>
   </si>
@@ -211,13 +211,19 @@
   </si>
   <si>
     <t>Websites</t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,6 +248,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -280,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -316,20 +329,34 @@
     <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -367,7 +394,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -401,6 +428,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -435,9 +463,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -610,20 +639,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1">
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>50</v>
       </c>
@@ -633,8 +665,11 @@
       <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="10" customFormat="1">
+      <c r="D1" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>60</v>
       </c>
@@ -646,12 +681,13 @@
         <f>SUM(B3:B1048576)*1.2</f>
         <v>57.599999999999994</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11"/>
+      <c r="E2" s="12">
         <f>C2/B2</f>
         <v>0.87272727272727268</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -662,7 +698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -673,18 +709,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="30">
+      <c r="D5" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -695,40 +734,47 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="45">
-      <c r="A8" s="1" t="s">
+      <c r="D7" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="14">
+        <v>1</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+      <c r="D8" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -736,7 +782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
@@ -747,18 +793,21 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="14">
+        <v>1</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="30">
+      <c r="D12" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -769,7 +818,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -780,7 +829,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -791,18 +840,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="14">
+        <v>1</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="30">
+      <c r="D16" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -813,7 +865,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45">
+    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
@@ -824,7 +876,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -832,7 +884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -843,7 +895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -851,7 +903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>61</v>
       </c>
@@ -859,7 +911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>63</v>
       </c>
@@ -867,7 +919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
@@ -880,19 +932,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1">
+    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>50</v>
       </c>
@@ -903,17 +955,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -921,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -929,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -937,27 +989,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -965,27 +1017,27 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -997,19 +1049,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1">
+    <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
@@ -1023,7 +1075,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>

</xml_diff>